<commit_message>
Fix Excel export template integration
</commit_message>
<xml_diff>
--- a/public/xlsx/health-offer-template.xlsx
+++ b/public/xlsx/health-offer-template.xlsx
@@ -9,16 +9,11 @@
   </sheets>
   <definedNames/>
   <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="bHo+w6fnazgfy76vZM3W7Fil1iGs8DzBcXu1y4PtuEU="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="98">
   <si>
     <t>APZĪMĒJUMI</t>
   </si>
@@ -156,6 +151,9 @@
     <t>Piemaksa par plastikāta kartēm, EUR</t>
   </si>
   <si>
+    <t>ir iekļauts</t>
+  </si>
+  <si>
     <t>Papildus programmas</t>
   </si>
   <si>
@@ -171,18 +169,6 @@
     <t>Vakcinācija pret ērčiem un gripu</t>
   </si>
   <si>
-    <t>Vakcinācija jebkura</t>
-  </si>
-  <si>
-    <t>ir iekļauts</t>
-  </si>
-  <si>
-    <t>Fizikālās terapijas procedūras, limits 10 reizes, 100% vai limits, EUR</t>
-  </si>
-  <si>
-    <t>Maksas grūtnieču aprūpem limits EUR</t>
-  </si>
-  <si>
     <t>Ambulatorā rehabilitācija, limtis EUR</t>
   </si>
   <si>
@@ -202,6 +188,9 @@
   </si>
   <si>
     <t>10 (1000 EUR limits)</t>
+  </si>
+  <si>
+    <t>Maksas stacionārie pakalpojumi, limits EUR (pp)</t>
   </si>
   <si>
     <t>Maksas operācijas, limits EUR</t>
@@ -656,7 +645,7 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -733,93 +722,90 @@
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="17" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="4" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="17" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="4" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -827,6 +813,9 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1088,6 +1077,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="33.43"/>
     <col customWidth="1" min="2" max="2" width="15.71"/>
+    <col customWidth="1" min="3" max="6" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
@@ -1330,7 +1320,7 @@
       </c>
       <c r="B32" s="25"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" ht="30.0" customHeight="1">
       <c r="A33" s="23" t="s">
         <v>38</v>
       </c>
@@ -1366,8 +1356,8 @@
       <c r="A37" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="5">
-        <v>5.0</v>
+      <c r="B37" s="26" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="38" ht="12.0" customHeight="1">
@@ -1376,13 +1366,13 @@
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B39" s="30"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B40" s="23" t="s">
         <v>20</v>
@@ -1390,1081 +1380,1784 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" ht="15.0" customHeight="1">
       <c r="A42" s="23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B42" s="23"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="23" t="s">
-        <v>50</v>
+      <c r="A43" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="25"/>
+      <c r="B44" s="26" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" s="33"/>
+        <v>54</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="12" t="s">
-        <v>54</v>
+      <c r="A46" s="33" t="s">
+        <v>56</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="12" t="s">
-        <v>55</v>
+      <c r="A47" s="34" t="s">
+        <v>58</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="34" t="s">
-        <v>57</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" ht="10.5" customHeight="1">
+      <c r="A48" s="24" t="s">
+        <v>59</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="35" t="s">
-        <v>59</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" ht="12.0" customHeight="1">
+      <c r="A49" s="24" t="s">
+        <v>60</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B50" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" ht="10.5" customHeight="1">
-      <c r="A51" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" ht="12.0" customHeight="1">
+      <c r="A50" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B51" s="25"/>
+      <c r="B50" s="36"/>
+    </row>
+    <row r="51" ht="12.0" customHeight="1">
+      <c r="A51" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="38"/>
     </row>
     <row r="52" ht="12.0" customHeight="1">
-      <c r="A52" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B52" s="25"/>
-    </row>
-    <row r="53" ht="12.0" customHeight="1">
-      <c r="A53" s="36" t="s">
+      <c r="A52" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="37"/>
-    </row>
-    <row r="54" ht="12.0" customHeight="1">
-      <c r="A54" s="38" t="s">
+      <c r="B52" s="38"/>
+    </row>
+    <row r="53" ht="12.75" customHeight="1">
+      <c r="A53" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="39"/>
-    </row>
-    <row r="55" ht="12.0" customHeight="1">
-      <c r="A55" s="38" t="s">
+      <c r="B53" s="4"/>
+    </row>
+    <row r="54" ht="12.75" customHeight="1">
+      <c r="A54" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="39"/>
+      <c r="B54" s="4"/>
+    </row>
+    <row r="55" ht="12.75" customHeight="1">
+      <c r="A55" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="40" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="B56" s="4"/>
+      <c r="A56" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="42" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B57" s="4"/>
+      <c r="A57" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" s="44">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="58" ht="12.75" customHeight="1">
-      <c r="A58" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" s="42" t="s">
-        <v>69</v>
+      <c r="A58" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="44">
+        <v>1.0</v>
       </c>
     </row>
     <row r="59" ht="12.75" customHeight="1">
       <c r="A59" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B59" s="44" t="s">
-        <v>25</v>
+        <v>71</v>
+      </c>
+      <c r="B59" s="44">
+        <v>1.0</v>
       </c>
     </row>
     <row r="60" ht="12.75" customHeight="1">
-      <c r="A60" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="B60" s="46">
+      <c r="A60" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" s="44">
         <v>1.0</v>
       </c>
     </row>
-    <row r="61" ht="12.75" customHeight="1">
-      <c r="A61" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="B61" s="46">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="62" ht="12.75" customHeight="1">
-      <c r="A62" s="45" t="s">
+    <row r="61" ht="12.0" customHeight="1">
+      <c r="A61" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B62" s="46">
-        <v>1.0</v>
-      </c>
+      <c r="B61" s="36"/>
+    </row>
+    <row r="62" ht="12.0" customHeight="1">
+      <c r="A62" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62" s="38"/>
     </row>
     <row r="63" ht="12.75" customHeight="1">
       <c r="A63" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="B63" s="46">
-        <v>1.0</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B63" s="4"/>
     </row>
     <row r="64" ht="12.0" customHeight="1">
-      <c r="A64" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="B64" s="37"/>
+      <c r="A64" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64" s="47"/>
     </row>
     <row r="65" ht="12.0" customHeight="1">
-      <c r="A65" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B65" s="39"/>
-    </row>
-    <row r="66" ht="12.75" customHeight="1">
-      <c r="A66" s="47" t="s">
+      <c r="A65" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="B66" s="4"/>
+      <c r="B65" s="49"/>
+    </row>
+    <row r="66" ht="12.0" customHeight="1">
+      <c r="A66" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66" s="50"/>
     </row>
     <row r="67" ht="12.0" customHeight="1">
       <c r="A67" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="B67" s="49"/>
-    </row>
-    <row r="68" ht="12.0" customHeight="1">
-      <c r="A68" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="B68" s="51"/>
-    </row>
-    <row r="69" ht="12.0" customHeight="1">
-      <c r="A69" s="50" t="s">
+      <c r="B67" s="50"/>
+    </row>
+    <row r="68" ht="12.75" customHeight="1">
+      <c r="A68" s="51" t="s">
         <v>80</v>
       </c>
+      <c r="B68" s="52"/>
+    </row>
+    <row r="69" ht="12.75" customHeight="1">
+      <c r="A69" s="53" t="s">
+        <v>81</v>
+      </c>
       <c r="B69" s="52"/>
     </row>
-    <row r="70" ht="12.0" customHeight="1">
-      <c r="A70" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="B70" s="52"/>
+    <row r="70" ht="24.75" customHeight="1">
+      <c r="A70" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" s="55"/>
     </row>
     <row r="71" ht="12.75" customHeight="1">
-      <c r="A71" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="B71" s="54"/>
+      <c r="A71" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71" s="4"/>
     </row>
     <row r="72" ht="12.75" customHeight="1">
-      <c r="A72" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="B72" s="54"/>
-    </row>
-    <row r="73" ht="24.75" customHeight="1">
-      <c r="A73" s="56" t="s">
+      <c r="A72" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="B73" s="57"/>
+      <c r="B72" s="56"/>
+    </row>
+    <row r="73" ht="12.75" customHeight="1">
+      <c r="A73" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73" s="49"/>
     </row>
     <row r="74" ht="12.75" customHeight="1">
-      <c r="A74" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="B74" s="4"/>
+      <c r="A74" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" s="57"/>
     </row>
     <row r="75" ht="12.75" customHeight="1">
-      <c r="A75" s="56" t="s">
+      <c r="A75" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="B75" s="58"/>
+      <c r="B75" s="57"/>
     </row>
     <row r="76" ht="12.75" customHeight="1">
-      <c r="A76" s="55" t="s">
+      <c r="A76" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="B76" s="51"/>
-    </row>
-    <row r="77" ht="12.75" customHeight="1">
-      <c r="A77" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="B77" s="59"/>
+      <c r="B76" s="52"/>
+    </row>
+    <row r="77" ht="24.75" customHeight="1">
+      <c r="A77" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="B77" s="52"/>
     </row>
     <row r="78" ht="12.75" customHeight="1">
-      <c r="A78" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B78" s="59"/>
-    </row>
-    <row r="79" ht="12.75" customHeight="1">
-      <c r="A79" s="55" t="s">
+      <c r="A78" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="B79" s="54"/>
-    </row>
-    <row r="80" ht="24.75" customHeight="1">
-      <c r="A80" s="55" t="s">
-        <v>90</v>
-      </c>
-      <c r="B80" s="54"/>
-    </row>
-    <row r="81" ht="12.75" customHeight="1">
-      <c r="A81" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="B81" s="54"/>
+      <c r="B78" s="52"/>
+    </row>
+    <row r="79" ht="10.5" customHeight="1">
+      <c r="A79" s="28"/>
+      <c r="B79" s="52"/>
+    </row>
+    <row r="80" ht="10.5" customHeight="1">
+      <c r="A80" s="58"/>
+      <c r="B80" s="52"/>
+    </row>
+    <row r="81" ht="10.5" customHeight="1">
+      <c r="A81" s="59"/>
+      <c r="B81" s="52"/>
     </row>
     <row r="82" ht="10.5" customHeight="1">
-      <c r="A82" s="28"/>
-      <c r="B82" s="54"/>
+      <c r="A82" s="59"/>
+      <c r="B82" s="59"/>
     </row>
     <row r="83" ht="10.5" customHeight="1">
-      <c r="A83" s="60"/>
-      <c r="B83" s="54"/>
+      <c r="A83" s="59"/>
+      <c r="B83" s="59"/>
     </row>
     <row r="84" ht="10.5" customHeight="1">
-      <c r="A84" s="33"/>
-      <c r="B84" s="54"/>
+      <c r="A84" s="59"/>
+      <c r="B84" s="49"/>
     </row>
     <row r="85" ht="10.5" customHeight="1">
-      <c r="A85" s="33"/>
-      <c r="B85" s="33"/>
+      <c r="A85" s="57"/>
+      <c r="B85" s="50"/>
     </row>
     <row r="86" ht="10.5" customHeight="1">
-      <c r="A86" s="33"/>
-      <c r="B86" s="33"/>
+      <c r="A86" s="57"/>
+      <c r="B86" s="50"/>
     </row>
     <row r="87" ht="10.5" customHeight="1">
-      <c r="A87" s="33"/>
-      <c r="B87" s="51"/>
+      <c r="A87" s="57"/>
+      <c r="B87" s="50"/>
     </row>
     <row r="88" ht="10.5" customHeight="1">
-      <c r="A88" s="59"/>
+      <c r="A88" s="60"/>
       <c r="B88" s="52"/>
     </row>
     <row r="89" ht="10.5" customHeight="1">
-      <c r="A89" s="59"/>
+      <c r="A89" s="60"/>
       <c r="B89" s="52"/>
     </row>
     <row r="90" ht="10.5" customHeight="1">
-      <c r="A90" s="59"/>
+      <c r="A90" s="60"/>
       <c r="B90" s="52"/>
     </row>
     <row r="91" ht="10.5" customHeight="1">
-      <c r="A91" s="61"/>
-      <c r="B91" s="54"/>
+      <c r="A91" s="60"/>
+      <c r="B91" s="52"/>
     </row>
     <row r="92" ht="10.5" customHeight="1">
-      <c r="A92" s="61"/>
-      <c r="B92" s="54"/>
+      <c r="A92" s="60"/>
+      <c r="B92" s="52"/>
     </row>
     <row r="93" ht="10.5" customHeight="1">
-      <c r="A93" s="61"/>
-      <c r="B93" s="54"/>
+      <c r="A93" s="60"/>
+      <c r="B93" s="52"/>
     </row>
     <row r="94" ht="10.5" customHeight="1">
-      <c r="A94" s="61"/>
-      <c r="B94" s="54"/>
+      <c r="A94" s="58"/>
+      <c r="B94" s="61"/>
     </row>
     <row r="95" ht="10.5" customHeight="1">
-      <c r="A95" s="61"/>
-      <c r="B95" s="54"/>
+      <c r="A95" s="62"/>
+      <c r="B95" s="63"/>
     </row>
     <row r="96" ht="10.5" customHeight="1">
-      <c r="A96" s="61"/>
-      <c r="B96" s="54"/>
+      <c r="A96" s="62"/>
+      <c r="B96" s="63"/>
     </row>
     <row r="97" ht="10.5" customHeight="1">
-      <c r="A97" s="60"/>
-      <c r="B97" s="62"/>
+      <c r="A97" s="64"/>
+      <c r="B97" s="63"/>
     </row>
     <row r="98" ht="10.5" customHeight="1">
-      <c r="A98" s="63"/>
-      <c r="B98" s="32"/>
+      <c r="A98" s="60"/>
+      <c r="B98" s="52"/>
     </row>
     <row r="99" ht="10.5" customHeight="1">
-      <c r="A99" s="63"/>
-      <c r="B99" s="32"/>
+      <c r="A99" s="65"/>
+      <c r="B99" s="52"/>
     </row>
     <row r="100" ht="10.5" customHeight="1">
-      <c r="A100" s="64"/>
-      <c r="B100" s="32"/>
+      <c r="A100" s="66"/>
+      <c r="B100" s="52"/>
     </row>
     <row r="101" ht="10.5" customHeight="1">
-      <c r="A101" s="61"/>
-      <c r="B101" s="54"/>
+      <c r="A101" s="66"/>
+      <c r="B101" s="52"/>
     </row>
     <row r="102" ht="10.5" customHeight="1">
-      <c r="A102" s="65"/>
-      <c r="B102" s="54"/>
+      <c r="A102" s="66"/>
+      <c r="B102" s="52"/>
     </row>
     <row r="103" ht="10.5" customHeight="1">
       <c r="A103" s="66"/>
-      <c r="B103" s="54"/>
+      <c r="B103" s="52"/>
     </row>
     <row r="104" ht="10.5" customHeight="1">
-      <c r="A104" s="66"/>
-      <c r="B104" s="54"/>
+      <c r="A104" s="58"/>
+      <c r="B104" s="52"/>
     </row>
     <row r="105" ht="10.5" customHeight="1">
-      <c r="A105" s="66"/>
-      <c r="B105" s="54"/>
+      <c r="A105" s="59"/>
+      <c r="B105" s="59"/>
     </row>
     <row r="106" ht="10.5" customHeight="1">
-      <c r="A106" s="66"/>
-      <c r="B106" s="54"/>
+      <c r="A106" s="59"/>
+      <c r="B106" s="59"/>
     </row>
     <row r="107" ht="10.5" customHeight="1">
-      <c r="A107" s="60"/>
-      <c r="B107" s="54"/>
+      <c r="A107" s="59"/>
+      <c r="B107" s="49"/>
     </row>
     <row r="108" ht="10.5" customHeight="1">
-      <c r="A108" s="33"/>
-      <c r="B108" s="33"/>
+      <c r="A108" s="67"/>
+      <c r="B108" s="52"/>
     </row>
     <row r="109" ht="10.5" customHeight="1">
-      <c r="A109" s="33"/>
-      <c r="B109" s="33"/>
+      <c r="A109" s="57"/>
+      <c r="B109" s="52"/>
     </row>
     <row r="110" ht="10.5" customHeight="1">
-      <c r="A110" s="33"/>
-      <c r="B110" s="51"/>
+      <c r="A110" s="57"/>
+      <c r="B110" s="52"/>
     </row>
     <row r="111" ht="10.5" customHeight="1">
-      <c r="A111" s="67"/>
-      <c r="B111" s="54"/>
+      <c r="A111" s="57"/>
+      <c r="B111" s="52"/>
     </row>
     <row r="112" ht="10.5" customHeight="1">
-      <c r="A112" s="59"/>
-      <c r="B112" s="54"/>
+      <c r="A112" s="57"/>
+      <c r="B112" s="52"/>
     </row>
     <row r="113" ht="10.5" customHeight="1">
-      <c r="A113" s="59"/>
-      <c r="B113" s="54"/>
+      <c r="A113" s="57"/>
+      <c r="B113" s="52"/>
     </row>
     <row r="114" ht="10.5" customHeight="1">
-      <c r="A114" s="59"/>
-      <c r="B114" s="54"/>
+      <c r="A114" s="57"/>
+      <c r="B114" s="52"/>
     </row>
     <row r="115" ht="10.5" customHeight="1">
-      <c r="A115" s="59"/>
-      <c r="B115" s="54"/>
+      <c r="A115" s="57"/>
+      <c r="B115" s="52"/>
     </row>
     <row r="116" ht="10.5" customHeight="1">
-      <c r="A116" s="59"/>
-      <c r="B116" s="54"/>
+      <c r="A116" s="57"/>
+      <c r="B116" s="52"/>
     </row>
     <row r="117" ht="10.5" customHeight="1">
-      <c r="A117" s="59"/>
-      <c r="B117" s="54"/>
+      <c r="A117" s="57"/>
+      <c r="B117" s="52"/>
     </row>
     <row r="118" ht="10.5" customHeight="1">
-      <c r="A118" s="59"/>
-      <c r="B118" s="54"/>
+      <c r="A118" s="57"/>
+      <c r="B118" s="52"/>
     </row>
     <row r="119" ht="10.5" customHeight="1">
-      <c r="A119" s="59"/>
-      <c r="B119" s="54"/>
+      <c r="A119" s="60"/>
+      <c r="B119" s="52"/>
     </row>
     <row r="120" ht="10.5" customHeight="1">
-      <c r="A120" s="59"/>
-      <c r="B120" s="54"/>
+      <c r="A120" s="68"/>
+      <c r="B120" s="52"/>
     </row>
     <row r="121" ht="10.5" customHeight="1">
-      <c r="A121" s="59"/>
-      <c r="B121" s="54"/>
+      <c r="A121" s="57"/>
+      <c r="B121" s="50"/>
     </row>
     <row r="122" ht="10.5" customHeight="1">
-      <c r="A122" s="61"/>
-      <c r="B122" s="54"/>
+      <c r="A122" s="57"/>
+      <c r="B122" s="50"/>
     </row>
     <row r="123" ht="10.5" customHeight="1">
-      <c r="A123" s="68"/>
-      <c r="B123" s="54"/>
+      <c r="A123" s="57"/>
+      <c r="B123" s="52"/>
     </row>
     <row r="124" ht="10.5" customHeight="1">
-      <c r="A124" s="59"/>
+      <c r="A124" s="57"/>
       <c r="B124" s="52"/>
     </row>
     <row r="125" ht="10.5" customHeight="1">
-      <c r="A125" s="59"/>
+      <c r="A125" s="60"/>
       <c r="B125" s="52"/>
     </row>
     <row r="126" ht="10.5" customHeight="1">
-      <c r="A126" s="59"/>
-      <c r="B126" s="54"/>
+      <c r="A126" s="68"/>
+      <c r="B126" s="52"/>
     </row>
     <row r="127" ht="10.5" customHeight="1">
-      <c r="A127" s="59"/>
-      <c r="B127" s="54"/>
+      <c r="A127" s="57"/>
+      <c r="B127" s="50"/>
     </row>
     <row r="128" ht="10.5" customHeight="1">
-      <c r="A128" s="61"/>
-      <c r="B128" s="54"/>
+      <c r="A128" s="57"/>
+      <c r="B128" s="50"/>
     </row>
     <row r="129" ht="10.5" customHeight="1">
-      <c r="A129" s="68"/>
-      <c r="B129" s="54"/>
+      <c r="A129" s="60"/>
+      <c r="B129" s="52"/>
     </row>
     <row r="130" ht="10.5" customHeight="1">
-      <c r="A130" s="59"/>
+      <c r="A130" s="67"/>
       <c r="B130" s="52"/>
     </row>
     <row r="131" ht="10.5" customHeight="1">
-      <c r="A131" s="59"/>
+      <c r="A131" s="57"/>
       <c r="B131" s="52"/>
     </row>
     <row r="132" ht="10.5" customHeight="1">
-      <c r="A132" s="61"/>
-      <c r="B132" s="54"/>
+      <c r="A132" s="57"/>
+      <c r="B132" s="52"/>
     </row>
     <row r="133" ht="10.5" customHeight="1">
-      <c r="A133" s="67"/>
-      <c r="B133" s="54"/>
+      <c r="A133" s="57"/>
+      <c r="B133" s="52"/>
     </row>
     <row r="134" ht="10.5" customHeight="1">
-      <c r="A134" s="59"/>
-      <c r="B134" s="54"/>
+      <c r="A134" s="57"/>
+      <c r="B134" s="52"/>
     </row>
     <row r="135" ht="10.5" customHeight="1">
-      <c r="A135" s="59"/>
-      <c r="B135" s="54"/>
+      <c r="A135" s="57"/>
+      <c r="B135" s="52"/>
     </row>
     <row r="136" ht="10.5" customHeight="1">
-      <c r="A136" s="59"/>
-      <c r="B136" s="54"/>
+      <c r="A136" s="57"/>
+      <c r="B136" s="52"/>
     </row>
     <row r="137" ht="10.5" customHeight="1">
-      <c r="A137" s="59"/>
-      <c r="B137" s="54"/>
+      <c r="A137" s="57"/>
+      <c r="B137" s="69"/>
     </row>
     <row r="138" ht="10.5" customHeight="1">
-      <c r="A138" s="59"/>
-      <c r="B138" s="54"/>
+      <c r="A138" s="60"/>
+      <c r="B138" s="52"/>
     </row>
     <row r="139" ht="10.5" customHeight="1">
-      <c r="A139" s="59"/>
-      <c r="B139" s="54"/>
+      <c r="A139" s="67"/>
+      <c r="B139" s="52"/>
     </row>
     <row r="140" ht="10.5" customHeight="1">
-      <c r="A140" s="59"/>
-      <c r="B140" s="69"/>
+      <c r="A140" s="57"/>
+      <c r="B140" s="52"/>
     </row>
     <row r="141" ht="10.5" customHeight="1">
-      <c r="A141" s="61"/>
-      <c r="B141" s="54"/>
+      <c r="A141" s="57"/>
+      <c r="B141" s="52"/>
     </row>
     <row r="142" ht="10.5" customHeight="1">
-      <c r="A142" s="67"/>
-      <c r="B142" s="54"/>
+      <c r="A142" s="57"/>
+      <c r="B142" s="52"/>
     </row>
     <row r="143" ht="10.5" customHeight="1">
-      <c r="A143" s="59"/>
-      <c r="B143" s="54"/>
+      <c r="A143" s="57"/>
+      <c r="B143" s="52"/>
     </row>
     <row r="144" ht="10.5" customHeight="1">
-      <c r="A144" s="59"/>
-      <c r="B144" s="54"/>
+      <c r="A144" s="57"/>
+      <c r="B144" s="52"/>
     </row>
     <row r="145" ht="10.5" customHeight="1">
-      <c r="A145" s="59"/>
-      <c r="B145" s="54"/>
+      <c r="A145" s="57"/>
+      <c r="B145" s="52"/>
     </row>
     <row r="146" ht="10.5" customHeight="1">
-      <c r="A146" s="59"/>
-      <c r="B146" s="54"/>
+      <c r="A146" s="57"/>
+      <c r="B146" s="57"/>
     </row>
     <row r="147" ht="10.5" customHeight="1">
-      <c r="A147" s="59"/>
-      <c r="B147" s="54"/>
+      <c r="A147" s="57"/>
+      <c r="B147" s="52"/>
     </row>
     <row r="148" ht="10.5" customHeight="1">
-      <c r="A148" s="59"/>
-      <c r="B148" s="54"/>
+      <c r="A148" s="57"/>
+      <c r="B148" s="52"/>
     </row>
     <row r="149" ht="10.5" customHeight="1">
-      <c r="A149" s="59"/>
-      <c r="B149" s="59"/>
+      <c r="A149" s="57"/>
+      <c r="B149" s="52"/>
     </row>
     <row r="150" ht="10.5" customHeight="1">
-      <c r="A150" s="59"/>
-      <c r="B150" s="54"/>
+      <c r="A150" s="57"/>
+      <c r="B150" s="52"/>
     </row>
     <row r="151" ht="10.5" customHeight="1">
-      <c r="A151" s="59"/>
-      <c r="B151" s="54"/>
+      <c r="A151" s="57"/>
+      <c r="B151" s="52"/>
     </row>
     <row r="152" ht="10.5" customHeight="1">
-      <c r="A152" s="59"/>
-      <c r="B152" s="54"/>
+      <c r="A152" s="57"/>
+      <c r="B152" s="52"/>
     </row>
     <row r="153" ht="10.5" customHeight="1">
-      <c r="A153" s="59"/>
-      <c r="B153" s="54"/>
+      <c r="A153" s="57"/>
+      <c r="B153" s="52"/>
     </row>
     <row r="154" ht="10.5" customHeight="1">
-      <c r="A154" s="59"/>
-      <c r="B154" s="54"/>
+      <c r="A154" s="57"/>
+      <c r="B154" s="52"/>
     </row>
     <row r="155" ht="10.5" customHeight="1">
-      <c r="A155" s="59"/>
-      <c r="B155" s="54"/>
+      <c r="A155" s="57"/>
+      <c r="B155" s="52"/>
     </row>
     <row r="156" ht="10.5" customHeight="1">
-      <c r="A156" s="59"/>
-      <c r="B156" s="54"/>
+      <c r="A156" s="60"/>
+      <c r="B156" s="52"/>
     </row>
     <row r="157" ht="10.5" customHeight="1">
-      <c r="A157" s="59"/>
-      <c r="B157" s="54"/>
+      <c r="A157" s="65"/>
+      <c r="B157" s="52"/>
     </row>
     <row r="158" ht="10.5" customHeight="1">
-      <c r="A158" s="59"/>
-      <c r="B158" s="54"/>
+      <c r="A158" s="58"/>
+      <c r="B158" s="52"/>
     </row>
     <row r="159" ht="10.5" customHeight="1">
-      <c r="A159" s="61"/>
-      <c r="B159" s="54"/>
+      <c r="A159" s="59"/>
+      <c r="B159" s="59"/>
     </row>
     <row r="160" ht="10.5" customHeight="1">
-      <c r="A160" s="65"/>
-      <c r="B160" s="54"/>
+      <c r="A160" s="59"/>
+      <c r="B160" s="49"/>
     </row>
     <row r="161" ht="10.5" customHeight="1">
-      <c r="A161" s="60"/>
-      <c r="B161" s="54"/>
+      <c r="A161" s="57"/>
+      <c r="B161" s="50"/>
     </row>
     <row r="162" ht="10.5" customHeight="1">
-      <c r="A162" s="33"/>
-      <c r="B162" s="33"/>
+      <c r="A162" s="57"/>
+      <c r="B162" s="50"/>
     </row>
     <row r="163" ht="10.5" customHeight="1">
-      <c r="A163" s="33"/>
-      <c r="B163" s="51"/>
+      <c r="A163" s="57"/>
+      <c r="B163" s="50"/>
     </row>
     <row r="164" ht="10.5" customHeight="1">
-      <c r="A164" s="59"/>
+      <c r="A164" s="60"/>
       <c r="B164" s="52"/>
     </row>
     <row r="165" ht="10.5" customHeight="1">
-      <c r="A165" s="59"/>
+      <c r="A165" s="65"/>
       <c r="B165" s="52"/>
     </row>
     <row r="166" ht="10.5" customHeight="1">
-      <c r="A166" s="59"/>
+      <c r="A166" s="66"/>
       <c r="B166" s="52"/>
     </row>
     <row r="167" ht="10.5" customHeight="1">
-      <c r="A167" s="61"/>
-      <c r="B167" s="54"/>
+      <c r="A167" s="58"/>
+      <c r="B167" s="52"/>
     </row>
     <row r="168" ht="10.5" customHeight="1">
-      <c r="A168" s="65"/>
-      <c r="B168" s="54"/>
+      <c r="A168" s="59"/>
+      <c r="B168" s="52"/>
     </row>
     <row r="169" ht="10.5" customHeight="1">
-      <c r="A169" s="66"/>
-      <c r="B169" s="54"/>
+      <c r="A169" s="59"/>
+      <c r="B169" s="52"/>
     </row>
     <row r="170" ht="10.5" customHeight="1">
-      <c r="A170" s="60"/>
-      <c r="B170" s="54"/>
+      <c r="A170" s="59"/>
+      <c r="B170" s="49"/>
     </row>
     <row r="171" ht="10.5" customHeight="1">
-      <c r="A171" s="33"/>
-      <c r="B171" s="54"/>
+      <c r="A171" s="57"/>
+      <c r="B171" s="50"/>
     </row>
     <row r="172" ht="10.5" customHeight="1">
-      <c r="A172" s="33"/>
-      <c r="B172" s="54"/>
+      <c r="A172" s="57"/>
+      <c r="B172" s="50"/>
     </row>
     <row r="173" ht="10.5" customHeight="1">
-      <c r="A173" s="33"/>
-      <c r="B173" s="51"/>
+      <c r="A173" s="57"/>
+      <c r="B173" s="50"/>
     </row>
     <row r="174" ht="10.5" customHeight="1">
-      <c r="A174" s="59"/>
+      <c r="A174" s="60"/>
       <c r="B174" s="52"/>
     </row>
     <row r="175" ht="10.5" customHeight="1">
-      <c r="A175" s="59"/>
-      <c r="B175" s="52"/>
+      <c r="A175" s="58"/>
+      <c r="B175" s="61"/>
     </row>
     <row r="176" ht="10.5" customHeight="1">
-      <c r="A176" s="59"/>
-      <c r="B176" s="52"/>
+      <c r="A176" s="62"/>
+      <c r="B176" s="63"/>
     </row>
     <row r="177" ht="10.5" customHeight="1">
-      <c r="A177" s="61"/>
-      <c r="B177" s="54"/>
+      <c r="A177" s="62"/>
+      <c r="B177" s="63"/>
     </row>
     <row r="178" ht="10.5" customHeight="1">
-      <c r="A178" s="60"/>
-      <c r="B178" s="62"/>
+      <c r="A178" s="64"/>
+      <c r="B178" s="63"/>
     </row>
     <row r="179" ht="10.5" customHeight="1">
-      <c r="A179" s="63"/>
-      <c r="B179" s="32"/>
+      <c r="A179" s="60"/>
+      <c r="B179" s="52"/>
     </row>
     <row r="180" ht="10.5" customHeight="1">
-      <c r="A180" s="63"/>
-      <c r="B180" s="32"/>
+      <c r="A180" s="70"/>
+      <c r="B180" s="52"/>
     </row>
     <row r="181" ht="10.5" customHeight="1">
-      <c r="A181" s="64"/>
-      <c r="B181" s="32"/>
+      <c r="A181" s="71"/>
+      <c r="B181" s="52"/>
     </row>
     <row r="182" ht="10.5" customHeight="1">
-      <c r="A182" s="61"/>
-      <c r="B182" s="54"/>
+      <c r="A182" s="58"/>
+      <c r="B182" s="52"/>
     </row>
     <row r="183" ht="10.5" customHeight="1">
-      <c r="A183" s="70"/>
-      <c r="B183" s="54"/>
+      <c r="A183" s="59"/>
+      <c r="B183" s="52"/>
     </row>
     <row r="184" ht="10.5" customHeight="1">
-      <c r="A184" s="71"/>
-      <c r="B184" s="54"/>
+      <c r="A184" s="59"/>
+      <c r="B184" s="52"/>
     </row>
     <row r="185" ht="10.5" customHeight="1">
-      <c r="A185" s="60"/>
-      <c r="B185" s="54"/>
+      <c r="A185" s="59"/>
+      <c r="B185" s="49"/>
     </row>
     <row r="186" ht="10.5" customHeight="1">
-      <c r="A186" s="33"/>
-      <c r="B186" s="54"/>
+      <c r="A186" s="57"/>
+      <c r="B186" s="52"/>
     </row>
     <row r="187" ht="10.5" customHeight="1">
-      <c r="A187" s="33"/>
-      <c r="B187" s="54"/>
+      <c r="A187" s="57"/>
+      <c r="B187" s="52"/>
     </row>
     <row r="188" ht="10.5" customHeight="1">
-      <c r="A188" s="33"/>
-      <c r="B188" s="51"/>
+      <c r="A188" s="57"/>
+      <c r="B188" s="52"/>
     </row>
     <row r="189" ht="10.5" customHeight="1">
-      <c r="A189" s="59"/>
-      <c r="B189" s="54"/>
+      <c r="A189" s="57"/>
+      <c r="B189" s="52"/>
     </row>
     <row r="190" ht="10.5" customHeight="1">
-      <c r="A190" s="59"/>
-      <c r="B190" s="54"/>
+      <c r="A190" s="57"/>
+      <c r="B190" s="52"/>
     </row>
     <row r="191" ht="10.5" customHeight="1">
-      <c r="A191" s="59"/>
-      <c r="B191" s="54"/>
+      <c r="A191" s="57"/>
+      <c r="B191" s="52"/>
     </row>
     <row r="192" ht="10.5" customHeight="1">
-      <c r="A192" s="59"/>
-      <c r="B192" s="54"/>
+      <c r="A192" s="57"/>
+      <c r="B192" s="52"/>
     </row>
     <row r="193" ht="10.5" customHeight="1">
-      <c r="A193" s="59"/>
-      <c r="B193" s="54"/>
+      <c r="A193" s="60"/>
+      <c r="B193" s="52"/>
     </row>
     <row r="194" ht="10.5" customHeight="1">
-      <c r="A194" s="59"/>
-      <c r="B194" s="54"/>
+      <c r="A194" s="70"/>
+      <c r="B194" s="52"/>
     </row>
     <row r="195" ht="10.5" customHeight="1">
       <c r="A195" s="59"/>
-      <c r="B195" s="54"/>
+      <c r="B195" s="52"/>
     </row>
     <row r="196" ht="10.5" customHeight="1">
-      <c r="A196" s="61"/>
-      <c r="B196" s="54"/>
+      <c r="A196" s="58"/>
+      <c r="B196" s="52"/>
     </row>
     <row r="197" ht="10.5" customHeight="1">
-      <c r="A197" s="70"/>
-      <c r="B197" s="54"/>
+      <c r="A197" s="59"/>
+      <c r="B197" s="52"/>
     </row>
     <row r="198" ht="10.5" customHeight="1">
-      <c r="A198" s="33"/>
-      <c r="B198" s="54"/>
+      <c r="A198" s="59"/>
+      <c r="B198" s="52"/>
     </row>
     <row r="199" ht="10.5" customHeight="1">
-      <c r="A199" s="60"/>
-      <c r="B199" s="54"/>
+      <c r="A199" s="59"/>
+      <c r="B199" s="52"/>
     </row>
     <row r="200" ht="10.5" customHeight="1">
-      <c r="A200" s="33"/>
-      <c r="B200" s="54"/>
+      <c r="A200" s="59"/>
+      <c r="B200" s="52"/>
     </row>
     <row r="201" ht="10.5" customHeight="1">
-      <c r="A201" s="33"/>
-      <c r="B201" s="54"/>
+      <c r="A201" s="59"/>
+      <c r="B201" s="52"/>
     </row>
     <row r="202" ht="10.5" customHeight="1">
-      <c r="A202" s="33"/>
-      <c r="B202" s="54"/>
+      <c r="A202" s="57"/>
+      <c r="B202" s="50"/>
     </row>
     <row r="203" ht="10.5" customHeight="1">
-      <c r="A203" s="33"/>
-      <c r="B203" s="54"/>
+      <c r="A203" s="57"/>
+      <c r="B203" s="50"/>
     </row>
     <row r="204" ht="10.5" customHeight="1">
-      <c r="A204" s="33"/>
-      <c r="B204" s="54"/>
+      <c r="A204" s="57"/>
+      <c r="B204" s="52"/>
     </row>
     <row r="205" ht="10.5" customHeight="1">
-      <c r="A205" s="59"/>
-      <c r="B205" s="52"/>
+      <c r="A205" s="57"/>
+      <c r="B205" s="50"/>
     </row>
     <row r="206" ht="10.5" customHeight="1">
-      <c r="A206" s="59"/>
+      <c r="A206" s="60"/>
       <c r="B206" s="52"/>
     </row>
     <row r="207" ht="10.5" customHeight="1">
       <c r="A207" s="59"/>
-      <c r="B207" s="54"/>
+      <c r="B207" s="52"/>
     </row>
     <row r="208" ht="10.5" customHeight="1">
-      <c r="A208" s="59"/>
-      <c r="B208" s="52"/>
+      <c r="A208" s="57"/>
+      <c r="B208" s="50"/>
     </row>
     <row r="209" ht="10.5" customHeight="1">
-      <c r="A209" s="61"/>
-      <c r="B209" s="54"/>
+      <c r="A209" s="57"/>
+      <c r="B209" s="50"/>
     </row>
     <row r="210" ht="10.5" customHeight="1">
-      <c r="A210" s="33"/>
-      <c r="B210" s="54"/>
+      <c r="A210" s="57"/>
+      <c r="B210" s="52"/>
     </row>
     <row r="211" ht="10.5" customHeight="1">
-      <c r="A211" s="59"/>
-      <c r="B211" s="52"/>
+      <c r="A211" s="57"/>
+      <c r="B211" s="50"/>
     </row>
     <row r="212" ht="10.5" customHeight="1">
-      <c r="A212" s="59"/>
+      <c r="A212" s="57"/>
       <c r="B212" s="52"/>
     </row>
     <row r="213" ht="10.5" customHeight="1">
-      <c r="A213" s="59"/>
-      <c r="B213" s="54"/>
+      <c r="A213" s="57"/>
+      <c r="B213" s="52"/>
     </row>
     <row r="214" ht="10.5" customHeight="1">
-      <c r="A214" s="59"/>
+      <c r="A214" s="57"/>
       <c r="B214" s="52"/>
     </row>
     <row r="215" ht="10.5" customHeight="1">
-      <c r="A215" s="59"/>
-      <c r="B215" s="54"/>
+      <c r="A215" s="63"/>
+      <c r="B215" s="52"/>
     </row>
     <row r="216" ht="10.5" customHeight="1">
-      <c r="A216" s="59"/>
-      <c r="B216" s="54"/>
+      <c r="A216" s="63"/>
+      <c r="B216" s="52"/>
     </row>
     <row r="217" ht="10.5" customHeight="1">
-      <c r="A217" s="59"/>
-      <c r="B217" s="54"/>
+      <c r="A217" s="63"/>
+      <c r="B217" s="52"/>
     </row>
     <row r="218" ht="10.5" customHeight="1">
-      <c r="A218" s="32"/>
-      <c r="B218" s="54"/>
+      <c r="A218" s="63"/>
+      <c r="B218" s="52"/>
     </row>
     <row r="219" ht="10.5" customHeight="1">
-      <c r="A219" s="32"/>
-      <c r="B219" s="54"/>
+      <c r="A219" s="58"/>
+      <c r="B219" s="61"/>
     </row>
     <row r="220" ht="10.5" customHeight="1">
-      <c r="A220" s="32"/>
-      <c r="B220" s="54"/>
+      <c r="A220" s="62"/>
+      <c r="B220" s="63"/>
     </row>
     <row r="221" ht="10.5" customHeight="1">
-      <c r="A221" s="32"/>
-      <c r="B221" s="54"/>
+      <c r="A221" s="62"/>
+      <c r="B221" s="63"/>
     </row>
     <row r="222" ht="10.5" customHeight="1">
-      <c r="A222" s="60"/>
-      <c r="B222" s="62"/>
+      <c r="A222" s="64"/>
+      <c r="B222" s="63"/>
     </row>
     <row r="223" ht="10.5" customHeight="1">
-      <c r="A223" s="63"/>
-      <c r="B223" s="32"/>
+      <c r="A223" s="60"/>
+      <c r="B223" s="52"/>
     </row>
     <row r="224" ht="10.5" customHeight="1">
-      <c r="A224" s="63"/>
-      <c r="B224" s="32"/>
+      <c r="A224" s="70"/>
+      <c r="B224" s="52"/>
     </row>
     <row r="225" ht="10.5" customHeight="1">
-      <c r="A225" s="64"/>
-      <c r="B225" s="32"/>
+      <c r="A225" s="59"/>
+      <c r="B225" s="52"/>
     </row>
     <row r="226" ht="10.5" customHeight="1">
-      <c r="A226" s="61"/>
-      <c r="B226" s="54"/>
+      <c r="A226" s="58"/>
+      <c r="B226" s="52"/>
     </row>
     <row r="227" ht="10.5" customHeight="1">
-      <c r="A227" s="70"/>
-      <c r="B227" s="54"/>
+      <c r="A227" s="59"/>
+      <c r="B227" s="52"/>
     </row>
     <row r="228" ht="10.5" customHeight="1">
-      <c r="A228" s="33"/>
-      <c r="B228" s="54"/>
+      <c r="A228" s="72"/>
+      <c r="B228" s="52"/>
     </row>
     <row r="229" ht="10.5" customHeight="1">
-      <c r="A229" s="60"/>
-      <c r="B229" s="54"/>
+      <c r="A229" s="59"/>
+      <c r="B229" s="52"/>
     </row>
     <row r="230" ht="10.5" customHeight="1">
-      <c r="A230" s="33"/>
-      <c r="B230" s="54"/>
+      <c r="A230" s="59"/>
+      <c r="B230" s="52"/>
     </row>
     <row r="231" ht="10.5" customHeight="1">
-      <c r="A231" s="72"/>
-      <c r="B231" s="54"/>
+      <c r="A231" s="57"/>
+      <c r="B231" s="52"/>
     </row>
     <row r="232" ht="10.5" customHeight="1">
-      <c r="A232" s="33"/>
-      <c r="B232" s="54"/>
+      <c r="A232" s="57"/>
+      <c r="B232" s="52"/>
     </row>
     <row r="233" ht="10.5" customHeight="1">
-      <c r="A233" s="33"/>
-      <c r="B233" s="54"/>
+      <c r="A233" s="57"/>
+      <c r="B233" s="52"/>
     </row>
     <row r="234" ht="10.5" customHeight="1">
-      <c r="A234" s="59"/>
-      <c r="B234" s="54"/>
+      <c r="A234" s="57"/>
+      <c r="B234" s="52"/>
     </row>
     <row r="235" ht="10.5" customHeight="1">
-      <c r="A235" s="59"/>
-      <c r="B235" s="54"/>
+      <c r="A235" s="57"/>
+      <c r="B235" s="52"/>
     </row>
     <row r="236" ht="10.5" customHeight="1">
-      <c r="A236" s="59"/>
-      <c r="B236" s="54"/>
+      <c r="A236" s="57"/>
+      <c r="B236" s="52"/>
     </row>
     <row r="237" ht="10.5" customHeight="1">
-      <c r="A237" s="59"/>
-      <c r="B237" s="54"/>
+      <c r="A237" s="60"/>
+      <c r="B237" s="52"/>
     </row>
     <row r="238" ht="10.5" customHeight="1">
-      <c r="A238" s="59"/>
-      <c r="B238" s="54"/>
+      <c r="A238" s="65"/>
+      <c r="B238" s="52"/>
     </row>
     <row r="239" ht="10.5" customHeight="1">
-      <c r="A239" s="59"/>
-      <c r="B239" s="54"/>
+      <c r="A239" s="66"/>
+      <c r="B239" s="52"/>
     </row>
     <row r="240" ht="10.5" customHeight="1">
-      <c r="A240" s="61"/>
-      <c r="B240" s="54"/>
+      <c r="A240" s="66"/>
+      <c r="B240" s="52"/>
     </row>
     <row r="241" ht="10.5" customHeight="1">
-      <c r="A241" s="65"/>
-      <c r="B241" s="54"/>
+      <c r="A241" s="59"/>
+      <c r="B241" s="52"/>
     </row>
     <row r="242" ht="10.5" customHeight="1">
-      <c r="A242" s="66"/>
-      <c r="B242" s="54"/>
+      <c r="A242" s="72"/>
+      <c r="B242" s="52"/>
     </row>
     <row r="243" ht="10.5" customHeight="1">
-      <c r="A243" s="66"/>
-      <c r="B243" s="54"/>
+      <c r="A243" s="58"/>
+      <c r="B243" s="52"/>
     </row>
     <row r="244" ht="10.5" customHeight="1">
-      <c r="A244" s="33"/>
-      <c r="B244" s="54"/>
+      <c r="A244" s="60"/>
+      <c r="B244" s="52"/>
     </row>
     <row r="245" ht="10.5" customHeight="1">
-      <c r="A245" s="72"/>
-      <c r="B245" s="54"/>
+      <c r="A245" s="57"/>
+      <c r="B245" s="52"/>
     </row>
     <row r="246" ht="10.5" customHeight="1">
-      <c r="A246" s="60"/>
-      <c r="B246" s="54"/>
+      <c r="A246" s="57"/>
+      <c r="B246" s="52"/>
     </row>
     <row r="247" ht="10.5" customHeight="1">
-      <c r="A247" s="61"/>
-      <c r="B247" s="54"/>
+      <c r="A247" s="57"/>
+      <c r="B247" s="52"/>
     </row>
     <row r="248" ht="10.5" customHeight="1">
-      <c r="A248" s="59"/>
-      <c r="B248" s="54"/>
+      <c r="A248" s="60"/>
+      <c r="B248" s="52"/>
     </row>
     <row r="249" ht="10.5" customHeight="1">
-      <c r="A249" s="59"/>
-      <c r="B249" s="54"/>
+      <c r="A249" s="57"/>
+      <c r="B249" s="52"/>
     </row>
     <row r="250" ht="10.5" customHeight="1">
-      <c r="A250" s="59"/>
-      <c r="B250" s="54"/>
+      <c r="A250" s="57"/>
+      <c r="B250" s="52"/>
     </row>
     <row r="251" ht="10.5" customHeight="1">
-      <c r="A251" s="61"/>
-      <c r="B251" s="54"/>
+      <c r="A251" s="57"/>
+      <c r="B251" s="52"/>
     </row>
     <row r="252" ht="10.5" customHeight="1">
-      <c r="A252" s="59"/>
-      <c r="B252" s="54"/>
+      <c r="A252" s="57"/>
+      <c r="B252" s="52"/>
     </row>
     <row r="253" ht="10.5" customHeight="1">
-      <c r="A253" s="59"/>
-      <c r="B253" s="54"/>
+      <c r="A253" s="60"/>
+      <c r="B253" s="52"/>
     </row>
     <row r="254" ht="10.5" customHeight="1">
-      <c r="A254" s="59"/>
-      <c r="B254" s="54"/>
+      <c r="A254" s="60"/>
+      <c r="B254" s="52"/>
     </row>
     <row r="255" ht="10.5" customHeight="1">
-      <c r="A255" s="59"/>
-      <c r="B255" s="54"/>
+      <c r="A255" s="60"/>
+      <c r="B255" s="52"/>
     </row>
     <row r="256" ht="10.5" customHeight="1">
-      <c r="A256" s="61"/>
-      <c r="B256" s="54"/>
+      <c r="A256" s="60"/>
+      <c r="B256" s="52"/>
     </row>
     <row r="257" ht="10.5" customHeight="1">
-      <c r="A257" s="61"/>
-      <c r="B257" s="54"/>
+      <c r="A257" s="60"/>
+      <c r="B257" s="52"/>
     </row>
     <row r="258" ht="10.5" customHeight="1">
-      <c r="A258" s="61"/>
-      <c r="B258" s="54"/>
+      <c r="A258" s="60"/>
+      <c r="B258" s="52"/>
     </row>
     <row r="259" ht="10.5" customHeight="1">
-      <c r="A259" s="61"/>
-      <c r="B259" s="54"/>
+      <c r="A259" s="60"/>
+      <c r="B259" s="52"/>
     </row>
     <row r="260" ht="10.5" customHeight="1">
-      <c r="A260" s="61"/>
-      <c r="B260" s="54"/>
+      <c r="A260" s="60"/>
+      <c r="B260" s="52"/>
     </row>
     <row r="261" ht="10.5" customHeight="1">
-      <c r="A261" s="61"/>
-      <c r="B261" s="54"/>
+      <c r="A261" s="60"/>
+      <c r="B261" s="52"/>
     </row>
     <row r="262" ht="10.5" customHeight="1">
-      <c r="A262" s="61"/>
-      <c r="B262" s="54"/>
+      <c r="A262" s="60"/>
+      <c r="B262" s="52"/>
     </row>
     <row r="263" ht="10.5" customHeight="1">
-      <c r="A263" s="61"/>
-      <c r="B263" s="54"/>
+      <c r="A263" s="58"/>
+      <c r="B263" s="61"/>
     </row>
     <row r="264" ht="10.5" customHeight="1">
-      <c r="A264" s="61"/>
-      <c r="B264" s="54"/>
+      <c r="A264" s="62"/>
+      <c r="B264" s="63"/>
     </row>
     <row r="265" ht="10.5" customHeight="1">
-      <c r="A265" s="61"/>
-      <c r="B265" s="54"/>
+      <c r="A265" s="62"/>
+      <c r="B265" s="63"/>
     </row>
     <row r="266" ht="10.5" customHeight="1">
-      <c r="A266" s="60"/>
-      <c r="B266" s="62"/>
+      <c r="A266" s="64"/>
+      <c r="B266" s="63"/>
     </row>
     <row r="267" ht="10.5" customHeight="1">
-      <c r="A267" s="63"/>
-      <c r="B267" s="32"/>
+      <c r="A267" s="60"/>
+      <c r="B267" s="52"/>
     </row>
     <row r="268" ht="10.5" customHeight="1">
-      <c r="A268" s="63"/>
-      <c r="B268" s="32"/>
+      <c r="A268" s="65"/>
+      <c r="B268" s="52"/>
     </row>
     <row r="269" ht="10.5" customHeight="1">
-      <c r="A269" s="64"/>
-      <c r="B269" s="32"/>
+      <c r="A269" s="66"/>
+      <c r="B269" s="52"/>
     </row>
     <row r="270" ht="10.5" customHeight="1">
-      <c r="A270" s="61"/>
-      <c r="B270" s="54"/>
+      <c r="A270" s="66"/>
+      <c r="B270" s="52"/>
     </row>
     <row r="271" ht="10.5" customHeight="1">
-      <c r="A271" s="65"/>
-      <c r="B271" s="54"/>
+      <c r="A271" s="58"/>
+      <c r="B271" s="52"/>
     </row>
     <row r="272" ht="10.5" customHeight="1">
-      <c r="A272" s="66"/>
-      <c r="B272" s="54"/>
+      <c r="A272" s="73"/>
+      <c r="B272" s="52"/>
     </row>
     <row r="273" ht="10.5" customHeight="1">
-      <c r="A273" s="66"/>
-      <c r="B273" s="54"/>
+      <c r="A273" s="59"/>
+      <c r="B273" s="52"/>
     </row>
     <row r="274" ht="10.5" customHeight="1">
-      <c r="A274" s="60"/>
-      <c r="B274" s="54"/>
+      <c r="A274" s="63"/>
+      <c r="B274" s="52"/>
     </row>
     <row r="275" ht="10.5" customHeight="1">
-      <c r="A275" s="73"/>
-      <c r="B275" s="54"/>
+      <c r="A275" s="57"/>
+      <c r="B275" s="52"/>
     </row>
     <row r="276" ht="10.5" customHeight="1">
-      <c r="A276" s="33"/>
-      <c r="B276" s="54"/>
+      <c r="A276" s="57"/>
+      <c r="B276" s="52"/>
     </row>
     <row r="277" ht="10.5" customHeight="1">
-      <c r="A277" s="32"/>
-      <c r="B277" s="54"/>
+      <c r="A277" s="57"/>
+      <c r="B277" s="52"/>
     </row>
     <row r="278" ht="10.5" customHeight="1">
-      <c r="A278" s="59"/>
-      <c r="B278" s="54"/>
-    </row>
-    <row r="279" ht="10.5" customHeight="1">
-      <c r="A279" s="59"/>
-      <c r="B279" s="54"/>
-    </row>
-    <row r="280" ht="10.5" customHeight="1">
-      <c r="A280" s="59"/>
-      <c r="B280" s="54"/>
-    </row>
-    <row r="281" ht="10.5" customHeight="1">
-      <c r="A281" s="59"/>
-      <c r="B281" s="54"/>
-    </row>
+      <c r="A278" s="57"/>
+      <c r="B278" s="52"/>
+    </row>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A54"/>
-    <hyperlink r:id="rId2" ref="A55"/>
-    <hyperlink r:id="rId3" ref="A65"/>
+    <hyperlink r:id="rId1" ref="A51"/>
+    <hyperlink r:id="rId2" ref="A52"/>
+    <hyperlink r:id="rId3" ref="A62"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2484,7 +3177,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="6" width="8.86"/>
-    <col customWidth="1" min="7" max="26" width="10.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1">
@@ -2499,37 +3191,37 @@
     </row>
     <row r="3" ht="16.5" customHeight="1">
       <c r="A3" s="74" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="A4" s="74" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" ht="16.5" customHeight="1">
       <c r="A5" s="74" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" ht="16.5" customHeight="1">
       <c r="A7" s="74" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" ht="16.5" customHeight="1">
       <c r="A10" s="74" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" ht="16.5" customHeight="1">
       <c r="A12" s="74" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" ht="16.5" customHeight="1">
       <c r="A13" s="74" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" ht="16.5" customHeight="1">
@@ -2539,12 +3231,12 @@
     </row>
     <row r="15" ht="16.5" customHeight="1">
       <c r="A15" s="74" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" ht="16.5" customHeight="1">
       <c r="A16" s="74" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -3546,7 +4238,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="6" width="8.86"/>
-    <col customWidth="1" min="7" max="26" width="10.0"/>
   </cols>
   <sheetData>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>